<commit_message>
staging smoke test debugging
</commit_message>
<xml_diff>
--- a/Data Files/reviewLog.xlsx
+++ b/Data Files/reviewLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
   <si>
     <t>build</t>
   </si>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -598,7 +598,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>

</xml_diff>